<commit_message>
LOTS of fixes and improvements)))
</commit_message>
<xml_diff>
--- a/Ignition table - Standart.xlsx
+++ b/Ignition table - Standart.xlsx
@@ -169,11 +169,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137430144"/>
-        <c:axId val="137431680"/>
+        <c:axId val="244189056"/>
+        <c:axId val="244190592"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137430144"/>
+        <c:axId val="244189056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -182,7 +182,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137431680"/>
+        <c:crossAx val="244190592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -190,7 +190,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137431680"/>
+        <c:axId val="244190592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -201,7 +201,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137430144"/>
+        <c:crossAx val="244189056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -318,11 +318,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="137451776"/>
-        <c:axId val="137453568"/>
+        <c:axId val="244247552"/>
+        <c:axId val="244417280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="137451776"/>
+        <c:axId val="244247552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -331,7 +331,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137453568"/>
+        <c:crossAx val="244417280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -339,7 +339,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="137453568"/>
+        <c:axId val="244417280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -350,7 +350,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="137451776"/>
+        <c:crossAx val="244247552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1452,11 +1452,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="139287936"/>
-        <c:axId val="139293824"/>
+        <c:axId val="246645120"/>
+        <c:axId val="246646656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="139287936"/>
+        <c:axId val="246645120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1466,7 +1466,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139293824"/>
+        <c:crossAx val="246646656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1474,7 +1474,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="139293824"/>
+        <c:axId val="246646656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,7 +1485,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="139287936"/>
+        <c:crossAx val="246645120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1602,11 +1602,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="267178752"/>
-        <c:axId val="267180288"/>
+        <c:axId val="246656000"/>
+        <c:axId val="246674176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="267178752"/>
+        <c:axId val="246656000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1615,7 +1615,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267180288"/>
+        <c:crossAx val="246674176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1623,7 +1623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="267180288"/>
+        <c:axId val="246674176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1634,7 +1634,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="267178752"/>
+        <c:crossAx val="246656000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1722,14 +1722,14 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>885825</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>104774</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2072,7 +2072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E16" sqref="E1:E16"/>
     </sheetView>
   </sheetViews>

</xml_diff>